<commit_message>
Clean all the code and optimize
</commit_message>
<xml_diff>
--- a/doc/Journaux_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/doc/Journaux_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -152,16 +152,19 @@
     <t>Finalisation de la documentation avec Romain.</t>
   </si>
   <si>
-    <t>Modification de l'index</t>
-  </si>
-  <si>
     <t>Modification et tentative de compréhension de l'index avec le nouveau MCD.</t>
   </si>
   <si>
-    <t>Brainstorming et base de donnée</t>
+    <t>Brainstorming avec le groupe et création de la base de donnée.</t>
   </si>
   <si>
-    <t>Brainstorming avec le groupe et création de la base de donnée.</t>
+    <t>Ajout du purchase</t>
+  </si>
+  <si>
+    <t>Réfléction</t>
+  </si>
+  <si>
+    <t>Nouveau diagramme de flux</t>
   </si>
 </sst>
 </file>
@@ -299,42 +302,7 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color theme="7"/>
@@ -374,6 +342,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -386,6 +369,36 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -401,21 +414,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G1007" totalsRowShown="0" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G1007" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="A1:G1007"/>
   <sortState ref="A2:H3">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Date" dataDxfId="14"/>
-    <tableColumn id="2" name="Début" dataDxfId="13"/>
-    <tableColumn id="3" name="Fin" dataDxfId="12"/>
-    <tableColumn id="4" name="Durée" dataDxfId="0">
+    <tableColumn id="1" name="Date" dataDxfId="10"/>
+    <tableColumn id="2" name="Début" dataDxfId="9"/>
+    <tableColumn id="3" name="Fin" dataDxfId="8"/>
+    <tableColumn id="4" name="Durée" dataDxfId="7">
       <calculatedColumnFormula>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Thème" dataDxfId="11"/>
-    <tableColumn id="7" name="Description" dataDxfId="10"/>
-    <tableColumn id="8" name="Sources" dataDxfId="9"/>
+    <tableColumn id="5" name="Thème" dataDxfId="6"/>
+    <tableColumn id="7" name="Description" dataDxfId="5"/>
+    <tableColumn id="8" name="Sources" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -687,7 +700,7 @@
   <dimension ref="A1:L1099"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,10 +1502,10 @@
         <v>6.5277777777777768E-2</v>
       </c>
       <c r="E35" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>26</v>
@@ -1513,10 +1526,10 @@
         <v>0.10416666666666663</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>26</v>
@@ -1524,28 +1537,48 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <v>45085</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+        <v>45089</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.37847222222222227</v>
+      </c>
       <c r="D37" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="14"/>
+        <v>4.5138888888888951E-2</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
+      <c r="A38" s="7">
+        <v>45089</v>
+      </c>
+      <c r="B38" s="8">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.3923611111111111</v>
+      </c>
       <c r="D38" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -13509,28 +13542,44 @@
       <c r="G1099" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A34 A36:A1048576">
-    <cfRule type="timePeriod" dxfId="8" priority="7" timePeriod="today">
+  <conditionalFormatting sqref="A1:A34 A36 A38 A40:A1048576">
+    <cfRule type="timePeriod" dxfId="17" priority="11" timePeriod="today">
       <formula>FLOOR(A1,1)=TODAY()</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="7" priority="8" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="16" priority="12" timePeriod="yesterday">
       <formula>FLOOR(A1,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G10">
-    <cfRule type="timePeriod" dxfId="6" priority="5" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="15" priority="9" timePeriod="today">
       <formula>FLOOR(G9,1)=TODAY()</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="5" priority="6" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="14" priority="10" timePeriod="yesterday">
       <formula>FLOOR(G9,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="timePeriod" dxfId="4" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="13" priority="5" timePeriod="today">
       <formula>FLOOR(A35,1)=TODAY()</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="3" priority="2" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="12" priority="6" timePeriod="yesterday">
       <formula>FLOOR(A35,1)=TODAY()-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="timePeriod" dxfId="3" priority="3" timePeriod="today">
+      <formula>FLOOR(A37,1)=TODAY()</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="2" priority="4" timePeriod="yesterday">
+      <formula>FLOOR(A37,1)=TODAY()-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+      <formula>FLOOR(A39,1)=TODAY()</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="yesterday">
+      <formula>FLOOR(A39,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>